<commit_message>
data table and excel
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/HrmsTestData.xlsx
+++ b/src/test/resources/testdata/HrmsTestData.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10914"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/musaozdemir/Desktop/Eclipse-workspace/SyntxHrms/src/test/resources/testdata/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/musaozdemir/Desktop/Eclipse-workspace/CucumberFrameWork/src/test/resources/testdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{717101FB-FB67-654A-BC9B-474C73078F66}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7DC2626-3BFE-FE4A-9022-70A65DC73B39}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16260" xr2:uid="{8AF4A404-313A-6D48-AC57-E27FCF5E34E7}"/>
   </bookViews>
@@ -40,31 +40,31 @@
     <t>MiddleName</t>
   </si>
   <si>
-    <t>Johnn</t>
-  </si>
-  <si>
-    <t>Janen</t>
-  </si>
-  <si>
-    <t>Jamesn</t>
-  </si>
-  <si>
-    <t>Markn</t>
-  </si>
-  <si>
-    <t>Jan</t>
-  </si>
-  <si>
-    <t>Feb</t>
-  </si>
-  <si>
-    <t>Mar</t>
-  </si>
-  <si>
-    <t>Apr</t>
-  </si>
-  <si>
-    <t>Doeee</t>
+    <t>John</t>
+  </si>
+  <si>
+    <t>K</t>
+  </si>
+  <si>
+    <t>Doe</t>
+  </si>
+  <si>
+    <t>Katie</t>
+  </si>
+  <si>
+    <t>Ball</t>
+  </si>
+  <si>
+    <t>Donald</t>
+  </si>
+  <si>
+    <t>Trump</t>
+  </si>
+  <si>
+    <t>Mohammed</t>
+  </si>
+  <si>
+    <t>Salah</t>
   </si>
 </sst>
 </file>
@@ -427,7 +427,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="18.83203125" defaultRowHeight="34" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -454,40 +454,40 @@
         <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="34" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>8</v>
-      </c>
       <c r="C3" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="34" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="34" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>11</v>

</xml_diff>